<commit_message>
Remove SAMFIR from sample
</commit_message>
<xml_diff>
--- a/1 - Data Entry/Labor Force Survey/Menu/Sample.xlsx
+++ b/1 - Data Entry/Labor Force Survey/Menu/Sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Documents\GitHub\cspro-examples\1 - Data Entry\Labor Force Survey\Menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{575A9A38-9B60-45B9-AD6A-6A3CBD596C4F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11304" windowHeight="5796"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11304" windowHeight="5796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Homer Simpson</t>
   </si>
@@ -96,9 +97,6 @@
   </si>
   <si>
     <t>555-2393</t>
-  </si>
-  <si>
-    <t>SAMFIR</t>
   </si>
   <si>
     <t>Bob Census</t>
@@ -107,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="000"/>
     <numFmt numFmtId="165" formatCode="00"/>
@@ -185,7 +183,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -497,11 +495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +513,7 @@
     <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -555,11 +553,8 @@
       <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -599,11 +594,8 @@
       <c r="M2" s="3">
         <v>1</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -643,11 +635,8 @@
       <c r="M3" s="3">
         <v>1</v>
       </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -687,11 +676,8 @@
       <c r="M4" s="3">
         <v>1</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -720,7 +706,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>21</v>
@@ -730,9 +716,6 @@
       </c>
       <c r="M5" s="3">
         <v>1</v>
-      </c>
-      <c r="N5" s="1">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the Labor Force Survey example with new 7.3 features
</commit_message>
<xml_diff>
--- a/1 - Data Entry/Labor Force Survey/Menu/Sample.xlsx
+++ b/1 - Data Entry/Labor Force Survey/Menu/Sample.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Documents\GitHub\cspro-examples\1 - Data Entry\Labor Force Survey\Menu\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{575A9A38-9B60-45B9-AD6A-6A3CBD596C4F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23506912-FCF9-4872-A113-A576807DF7A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11304" windowHeight="5796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,22 +493,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -554,7 +547,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -595,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -636,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -677,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>

</xml_diff>